<commit_message>
docs: Update rubric checklist
</commit_message>
<xml_diff>
--- a/doc/Rubric.xlsx
+++ b/doc/Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\source\oliver-hh\udacity-projects\udacity-would-you-rather\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obrandt\source\oliver-hh\udacity-projects\udacity-would-you-rather\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19D0352-4798-4A4E-821F-7F46E3BE7423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58DE50D-23BB-4F80-81D4-ED3A59D45030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{D7FBC665-A57B-43DC-8516-9AF1E4F7DE45}"/>
+    <workbookView xWindow="-1995" yWindow="-20700" windowWidth="20775" windowHeight="19380" xr2:uid="{D7FBC665-A57B-43DC-8516-9AF1E4F7DE45}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>The application requires only npm install and npm start to install and launch.</t>
   </si>
@@ -177,31 +176,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. The details of the poll are available at </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>questions/:question_id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-  </si>
-  <si>
     <t>2. The application shows the text “Would You Rather” and has a form for creating two options.</t>
   </si>
   <si>
@@ -332,6 +306,33 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The details of the poll are available at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>questions/:question_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -475,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -495,24 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -557,6 +540,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -875,507 +879,514 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228B7648-A1A2-4356-B1B7-EC5EAAA4B88A}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.61328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="88.84375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.23046875" style="18"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="88.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="8"/>
-      <c r="B3" s="15" t="s">
+      <c r="D2" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
+      <c r="D3" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="10"/>
-      <c r="B5" s="12"/>
+      <c r="D4" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A6" s="10"/>
-      <c r="B6" s="12"/>
+      <c r="D5" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="10"/>
-      <c r="B7" s="12"/>
+      <c r="D6" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="11"/>
-      <c r="B8" s="8"/>
+      <c r="D7" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
+      <c r="D8" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="D9" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
+      <c r="D10" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="D11" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+      <c r="D12" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="12"/>
-      <c r="B14" s="8"/>
+      <c r="D13" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="102.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="12"/>
-      <c r="B15" s="17" t="s">
+      <c r="D14" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A16" s="12"/>
-      <c r="B16" s="7" t="s">
+      <c r="D15" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="D17" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="D18" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="D19" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="58.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="12"/>
-      <c r="B21" s="8"/>
+      <c r="D20" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="12"/>
-      <c r="B22" s="7" t="s">
+      <c r="D21" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="26" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="D22" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="D23" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="12"/>
-      <c r="B25" s="8"/>
+      <c r="D24" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="7" t="s">
+      <c r="D25" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="D26" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="12"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
+      <c r="B30" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" s="12"/>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="12"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" s="12"/>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="12"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="27"/>
+      <c r="B35" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35" s="12"/>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="12"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="28"/>
+      <c r="B37" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="58.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="8"/>
-      <c r="B37" s="13" t="s">
+      <c r="C37" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="87.9" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="9" t="s">
+      <c r="B38" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="C38" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="D38" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="58.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="10"/>
-      <c r="B39" s="20" t="s">
+      <c r="C39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="24"/>
+      <c r="B40" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="44.15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="10"/>
-      <c r="B40" s="20" t="s">
+      <c r="C40" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="25"/>
+      <c r="B41" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="44.15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="11"/>
-      <c r="B41" s="16" t="s">
+      <c r="C41" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" s="9" t="s">
+      <c r="B42" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="C42" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A43" s="10"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="25"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="11"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="16" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D44" xr:uid="{228B7648-A1A2-4356-B1B7-EC5EAAA4B88A}"/>
   <mergeCells count="14">
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B22:B25"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B30:B32"/>
@@ -1384,11 +1395,6 @@
     <mergeCell ref="A9:A37"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>